<commit_message>
Removing to-do, and updating spreadsheets to include all scenarios except AP12 and AP45, as well as removing sub-cases which exceed the 2% threshold
</commit_message>
<xml_diff>
--- a/input_files/plr_sheet.xlsx
+++ b/input_files/plr_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T\PycharmProjects\find-max-ssp\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEE2BCE-659F-4608-87AC-ABA9FCAAC60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1B7D2C-1455-4D33-8499-63F83678A100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-86" yWindow="0" windowWidth="16629" windowHeight="17880" xr2:uid="{41B3A736-BE96-4DDD-B183-15D4BB3D7DE1}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{41B3A736-BE96-4DDD-B183-15D4BB3D7DE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="288">
   <si>
     <t>AP12345_1</t>
   </si>
@@ -326,15 +326,6 @@
     <t>0.0599, 0.1547</t>
   </si>
   <si>
-    <t>AP124_5</t>
-  </si>
-  <si>
-    <t>1.7464, 5.0188</t>
-  </si>
-  <si>
-    <t>8.541, 24.8807</t>
-  </si>
-  <si>
     <t>AP125_1</t>
   </si>
   <si>
@@ -398,18 +389,6 @@
     <t>AP134_2</t>
   </si>
   <si>
-    <t>5.1636, 14.9803</t>
-  </si>
-  <si>
-    <t>0.0698, 0.1575</t>
-  </si>
-  <si>
-    <t>8.5696, 24.9279</t>
-  </si>
-  <si>
-    <t>17.0236, 49.681</t>
-  </si>
-  <si>
     <t>AP134_3</t>
   </si>
   <si>
@@ -419,9 +398,6 @@
     <t>0.057, 0.145</t>
   </si>
   <si>
-    <t>AP134_4</t>
-  </si>
-  <si>
     <t>0.0405, 0.0782</t>
   </si>
   <si>
@@ -521,9 +497,6 @@
     <t>AP245_4</t>
   </si>
   <si>
-    <t>AP245_5</t>
-  </si>
-  <si>
     <t>AP145_1</t>
   </si>
   <si>
@@ -542,9 +515,6 @@
     <t>AP235_2</t>
   </si>
   <si>
-    <t>AP235_3</t>
-  </si>
-  <si>
     <t>AP24_1</t>
   </si>
   <si>
@@ -833,21 +803,6 @@
     <t>0.6035, 1.1768</t>
   </si>
   <si>
-    <t>9.1558, 9.4552</t>
-  </si>
-  <si>
-    <t>0.1285, 0.3008</t>
-  </si>
-  <si>
-    <t>0.0905, 0.1999</t>
-  </si>
-  <si>
-    <t>0.0946, 0.2085</t>
-  </si>
-  <si>
-    <t>45.0725, 46.5342</t>
-  </si>
-  <si>
     <t>0.3116, 0.4774</t>
   </si>
   <si>
@@ -911,9 +866,6 @@
     <t>AP23_5</t>
   </si>
   <si>
-    <t>AP23_6</t>
-  </si>
-  <si>
     <t>AP35_1</t>
   </si>
   <si>
@@ -948,9 +900,6 @@
   </si>
   <si>
     <t>AP34_5</t>
-  </si>
-  <si>
-    <t>AP34_6</t>
   </si>
 </sst>
 </file>
@@ -1183,10 +1132,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1369,8 +1318,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25AC1611-B054-4585-A19F-1689A834AC99}" name="Table153" displayName="Table153" ref="A1:G85" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8">
-  <autoFilter ref="A1:G85" xr:uid="{25AC1611-B054-4585-A19F-1689A834AC99}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25AC1611-B054-4585-A19F-1689A834AC99}" name="Table153" displayName="Table153" ref="A1:G79" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8">
+  <autoFilter ref="A1:G79" xr:uid="{25AC1611-B054-4585-A19F-1689A834AC99}"/>
   <tableColumns count="7">
     <tableColumn id="2" xr3:uid="{47FA731A-B13C-430B-9BFB-1F7FE8DA1F6B}" name="Scenario_Name" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{3823FD61-7CBA-4931-9376-D6C992236347}" name="K_PLR" dataDxfId="5"/>
@@ -1701,43 +1650,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8950C5D0-3929-4E07-A5D6-544133507137}">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:XFD75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="14.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1760,7 +1709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1783,7 +1732,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1806,7 +1755,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1829,7 +1778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1852,7 +1801,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1875,7 +1824,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1898,7 +1847,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1921,7 +1870,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1944,7 +1893,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1967,7 +1916,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1990,7 +1939,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -2013,7 +1962,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -2036,7 +1985,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -2059,7 +2008,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -2082,7 +2031,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -2105,7 +2054,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -2128,7 +2077,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>82</v>
       </c>
@@ -2151,7 +2100,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -2174,7 +2123,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -2197,7 +2146,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>96</v>
       </c>
@@ -2205,45 +2154,45 @@
         <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="F22" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23" t="s">
         <v>98</v>
       </c>
-      <c r="G22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" t="s">
-        <v>101</v>
-      </c>
-      <c r="F23" t="s">
-        <v>102</v>
-      </c>
-      <c r="G23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -2251,45 +2200,45 @@
         <v>105</v>
       </c>
       <c r="C24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
         <v>59</v>
       </c>
-      <c r="D24" t="s">
+      <c r="F25" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" t="s">
         <v>60</v>
       </c>
-      <c r="E24" t="s">
-        <v>59</v>
-      </c>
-      <c r="F24" t="s">
-        <v>106</v>
-      </c>
-      <c r="G24" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" t="s">
-        <v>108</v>
-      </c>
-      <c r="C25" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" t="s">
-        <v>110</v>
-      </c>
-      <c r="G25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -2300,65 +2249,65 @@
         <v>113</v>
       </c>
       <c r="D26" t="s">
-        <v>49</v>
+        <v>114</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="F26" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="G26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
-        <v>114</v>
-      </c>
-      <c r="B27" t="s">
-        <v>115</v>
-      </c>
-      <c r="C27" t="s">
-        <v>116</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="G27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>117</v>
-      </c>
-      <c r="E27" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" t="s">
-        <v>93</v>
-      </c>
-      <c r="G27" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
-        <v>119</v>
       </c>
       <c r="B28" t="s">
         <v>120</v>
       </c>
       <c r="C28" t="s">
-        <v>109</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
         <v>121</v>
       </c>
       <c r="E28" t="s">
+        <v>122</v>
+      </c>
+      <c r="F28" t="s">
         <v>61</v>
-      </c>
-      <c r="F28" t="s">
-        <v>122</v>
       </c>
       <c r="G28" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>124</v>
       </c>
@@ -2366,1307 +2315,1169 @@
         <v>125</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D29" t="s">
         <v>126</v>
       </c>
       <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>127</v>
+      </c>
+      <c r="G29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A30" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F29" t="s">
-        <v>60</v>
-      </c>
-      <c r="G29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>127</v>
-      </c>
-      <c r="B30" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="E33" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D30" t="s">
-        <v>129</v>
-      </c>
-      <c r="E30" t="s">
-        <v>130</v>
-      </c>
-      <c r="F30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G30" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
-        <v>132</v>
-      </c>
-      <c r="B31" t="s">
-        <v>133</v>
-      </c>
-      <c r="C31" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" t="s">
-        <v>134</v>
-      </c>
-      <c r="E31" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" t="s">
-        <v>135</v>
-      </c>
-      <c r="G31" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>137</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A33" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>101</v>
-      </c>
       <c r="F33" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>59</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A35" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D35" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="F38" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A36" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>142</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>146</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A39" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A40" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A41" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A42" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="F42" s="7" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="6" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="C43" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G43" s="8" t="s">
+      <c r="E45" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A46" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A47" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A49" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A50" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A51" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A52" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A53" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A54" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A55" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A56" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A57" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A58" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A59" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A60" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A61" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C61" s="7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A44" s="6" t="s">
+      <c r="D61" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A62" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A63" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A64" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="G64" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A65" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D44" s="7" t="s">
+      <c r="B65" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A66" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G66" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A67" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A68" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A69" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A70" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A71" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A72" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A73" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A74" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A75" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="D75" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="E75" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="F75" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="G75" s="13" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A76" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G76" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A77" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D77" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E44" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A45" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A46" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A47" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A48" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A49" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G49" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A50" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G50" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A51" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A52" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A53" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G53" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A54" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="B54" s="12" t="s">
+      <c r="E77" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A78" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="B78" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C78" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="G78" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="D54" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="F54" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="G54" s="12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A55" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="C55" s="12" t="s">
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A79" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="B79" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="D55" s="12" t="s">
+      <c r="C79" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="G79" s="7" t="s">
         <v>199</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="F55" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A56" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="F56" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A57" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="F57" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="G57" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A58" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="C58" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="E58" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="F58" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A59" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="F59" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A60" s="12" t="s">
-        <v>282</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="F60" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="G60" s="12" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A61" s="12" t="s">
-        <v>283</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="F61" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="G61" s="12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A62" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="F62" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="G62" s="12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A63" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="F63" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="G63" s="12" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A64" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="C64" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="F64" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="G64" s="12" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A65" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="F65" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="G65" s="12" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A66" s="12" t="s">
-        <v>288</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="F66" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="G66" s="12" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A67" s="12" t="s">
-        <v>289</v>
-      </c>
-      <c r="B67" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>262</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="E67" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="F67" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G67" s="12" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="12" t="s">
-        <v>290</v>
-      </c>
-      <c r="B68" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="E68" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="F68" s="12" t="s">
-        <v>268</v>
-      </c>
-      <c r="G68" s="12" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="B69" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C69" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D69" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="E69" s="14" t="s">
-        <v>273</v>
-      </c>
-      <c r="F69" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="G69" s="15" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A70" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="G70" s="8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A71" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G71" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A72" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="B72" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="C72" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D72" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="F72" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="G72" s="11" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A73" s="12" t="s">
-        <v>296</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="C73" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="D73" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="E73" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="F73" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="G73" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A74" s="12" t="s">
-        <v>297</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="C74" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="D74" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="E74" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="F74" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="G74" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="C75" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D75" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="E75" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="F75" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="G75" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A76" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="B76" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="C76" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="D76" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="E76" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="F76" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="G76" s="12" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A77" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="C77" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="D77" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="E77" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="F77" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="G77" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A78" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="B78" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="C78" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="D78" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="E78" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="F78" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="G78" s="12" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A79" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="B79" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="C79" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="D79" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E79" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="F79" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="G79" s="12" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A80" s="12" t="s">
-        <v>303</v>
-      </c>
-      <c r="B80" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="C80" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="D80" s="12" t="s">
-        <v>268</v>
-      </c>
-      <c r="E80" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="F80" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="G80" s="12" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A81" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="B81" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="C81" s="15" t="s">
-        <v>275</v>
-      </c>
-      <c r="D81" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="E81" s="14" t="s">
-        <v>273</v>
-      </c>
-      <c r="F81" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="G81" s="14" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A82" s="12" t="s">
-        <v>292</v>
-      </c>
-      <c r="B82" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C82" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="D82" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="E82" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="F82" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G82" s="12" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A83" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="B83" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="C83" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="D83" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E83" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="F83" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="G83" s="12" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A84" s="12" t="s">
-        <v>294</v>
-      </c>
-      <c r="B84" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="C84" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="D84" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="E84" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="F84" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="G84" s="12" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A85" s="12" t="s">
-        <v>295</v>
-      </c>
-      <c r="B85" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="C85" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="D85" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="E85" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="F85" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="G85" s="12" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>